<commit_message>
data read and write to mysql
Pandas.to_sql is better.
</commit_message>
<xml_diff>
--- a/work_time_log.xlsx
+++ b/work_time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shuaiwang/Documents/2022/Search_Excel_Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6D8CD3-09C1-B64B-80CC-82738A9220E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B29F2D-14CC-CA4C-8A83-A794C7E86091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{F1C215AD-117D-E340-A4EC-8C5E914D94BD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Content</t>
   </si>
@@ -57,7 +57,14 @@
     <t>MySQL install and solve connect problem(Authentication plugin 'caching_sha2_password' is not supported)</t>
   </si>
   <si>
-    <t>import Excel to database by Python</t>
+    <t>import Excel to database by Python, tradition way by SQL language</t>
+  </si>
+  <si>
+    <t>Choose backend framework, Django VS Flask. Django is my choose, the reason is that both frameworks are new to me, but Django looks more mature platform. Django is similar to my previous enterprise development platform.</t>
+  </si>
+  <si>
+    <t>Two ways read and write data to mysql.
+df.to_sql is easier than mysql.connector. Later I will choose Pandas read and write on MySQL</t>
   </si>
 </sst>
 </file>
@@ -96,10 +103,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,16 +422,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85437E67-D083-D143-8800-0E0EB21C8F1F}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="34.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="49.1640625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -432,7 +443,7 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -470,7 +481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -484,7 +495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -493,6 +504,37 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44700</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44700</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>